<commit_message>
Results from July 22, 2020 04:06:40 PM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-22.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-22.xlsx
@@ -525,16 +525,16 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>44033</v>
+        <v>44034</v>
       </c>
       <c r="C2" t="n">
-        <v>28606</v>
+        <v>29588</v>
       </c>
       <c r="D2" t="n">
-        <v>758</v>
+        <v>764</v>
       </c>
       <c r="E2" t="n">
-        <v>3321</v>
+        <v>3491</v>
       </c>
       <c r="F2" t="n">
         <v>95</v>
@@ -543,7 +543,7 @@
         <v>0.12</v>
       </c>
       <c r="H2" t="n">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="I2" t="b">
         <v>1</v>
@@ -623,29 +623,29 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>44033</v>
+        <v>44034</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>219030</t>
+          <t>219128</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>18800</t>
+          <t>18803</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>33634</v>
+        <v>33790</v>
       </c>
       <c r="F4" t="n">
-        <v>5090</v>
+        <v>5239</v>
       </c>
       <c r="G4" t="n">
-        <v>30.09</v>
+        <v>30.07</v>
       </c>
       <c r="H4" t="n">
-        <v>30.47</v>
+        <v>30.43</v>
       </c>
       <c r="I4" t="b">
         <v>0</v>
@@ -654,10 +654,10 @@
         <v>1</v>
       </c>
       <c r="K4" t="n">
-        <v>111790</v>
+        <v>112360</v>
       </c>
       <c r="L4" t="n">
-        <v>16704</v>
+        <v>17217</v>
       </c>
       <c r="M4" t="n">
         <v>2049418</v>
@@ -776,25 +776,25 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>44033</v>
+        <v>44034</v>
       </c>
       <c r="C7" t="n">
-        <v>81944</v>
+        <v>84417</v>
       </c>
       <c r="D7" t="n">
-        <v>871</v>
+        <v>888</v>
       </c>
       <c r="E7" t="n">
-        <v>15752</v>
+        <v>16107</v>
       </c>
       <c r="F7" t="n">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="G7" t="n">
-        <v>19.22</v>
+        <v>19.08</v>
       </c>
       <c r="H7" t="n">
-        <v>36.17</v>
+        <v>35.92</v>
       </c>
       <c r="I7" t="b">
         <v>1</v>
@@ -823,32 +823,34 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>44033</v>
+        <v>44034</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>35012</t>
+          <t>35578</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>251</t>
+          <t>260</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>870</t>
+          <t>886</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>&lt;5</t>
+          <t>5</t>
         </is>
       </c>
       <c r="G8" t="n">
         <v>2.5</v>
       </c>
-      <c r="H8" t="inlineStr"/>
+      <c r="H8" t="n">
+        <v>1.92</v>
+      </c>
       <c r="I8" t="b">
         <v>1</v>
       </c>
@@ -876,25 +878,25 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>44033</v>
+        <v>44034</v>
       </c>
       <c r="C9" t="n">
-        <v>24060</v>
+        <v>24540</v>
       </c>
       <c r="D9" t="n">
-        <v>674</v>
+        <v>677</v>
       </c>
       <c r="E9" t="n">
-        <v>2012</v>
+        <v>2044</v>
       </c>
       <c r="F9" t="n">
         <v>92</v>
       </c>
       <c r="G9" t="n">
-        <v>12.71</v>
+        <v>12.43</v>
       </c>
       <c r="H9" t="n">
-        <v>14.63</v>
+        <v>14.69</v>
       </c>
       <c r="I9" t="b">
         <v>0</v>
@@ -903,10 +905,10 @@
         <v>1</v>
       </c>
       <c r="K9" t="n">
-        <v>15831</v>
+        <v>16446</v>
       </c>
       <c r="L9" t="n">
-        <v>628</v>
+        <v>632</v>
       </c>
       <c r="M9" t="n">
         <v>354112</v>
@@ -1076,16 +1078,16 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>44033</v>
+        <v>44034</v>
       </c>
       <c r="C13" t="n">
-        <v>17517</v>
+        <v>17828</v>
       </c>
       <c r="D13" t="n">
-        <v>588</v>
+        <v>591</v>
       </c>
       <c r="E13" t="n">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="n">
@@ -1209,25 +1211,25 @@
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>44033</v>
+        <v>44034</v>
       </c>
       <c r="C16" t="n">
-        <v>69075</v>
+        <v>70413</v>
       </c>
       <c r="D16" t="n">
-        <v>1268</v>
+        <v>1325</v>
       </c>
       <c r="E16" t="n">
-        <v>20540</v>
+        <v>20886</v>
       </c>
       <c r="F16" t="n">
-        <v>542</v>
+        <v>561</v>
       </c>
       <c r="G16" t="n">
-        <v>43.75</v>
+        <v>43.68</v>
       </c>
       <c r="H16" t="n">
-        <v>44.65</v>
+        <v>44.38</v>
       </c>
       <c r="I16" t="b">
         <v>0</v>
@@ -1236,10 +1238,10 @@
         <v>0</v>
       </c>
       <c r="K16" t="n">
-        <v>46948</v>
+        <v>47812</v>
       </c>
       <c r="L16" t="n">
-        <v>1214</v>
+        <v>1264</v>
       </c>
       <c r="M16" t="n">
         <v>1293186</v>
@@ -1362,25 +1364,25 @@
         </is>
       </c>
       <c r="B19" s="2" t="n">
-        <v>44032</v>
+        <v>44033</v>
       </c>
       <c r="C19" t="n">
-        <v>45524</v>
+        <v>47071</v>
       </c>
       <c r="D19" t="n">
-        <v>1389</v>
+        <v>1423</v>
       </c>
       <c r="E19" t="n">
-        <v>20429</v>
+        <v>20775</v>
       </c>
       <c r="F19" t="n">
-        <v>696</v>
+        <v>717</v>
       </c>
       <c r="G19" t="n">
-        <v>44.88</v>
+        <v>44.14</v>
       </c>
       <c r="H19" t="n">
-        <v>50.11</v>
+        <v>50.39</v>
       </c>
       <c r="I19" t="b">
         <v>1</v>
@@ -1409,25 +1411,25 @@
         </is>
       </c>
       <c r="B20" s="2" t="n">
-        <v>44033</v>
+        <v>44034</v>
       </c>
       <c r="C20" t="n">
-        <v>148683</v>
+        <v>150609</v>
       </c>
       <c r="D20" t="n">
-        <v>2918</v>
+        <v>2974</v>
       </c>
       <c r="E20" t="n">
-        <v>3207</v>
+        <v>3246</v>
       </c>
       <c r="F20" t="n">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G20" t="n">
-        <v>4.32</v>
+        <v>4.31</v>
       </c>
       <c r="H20" t="n">
-        <v>3.57</v>
+        <v>3.47</v>
       </c>
       <c r="I20" t="b">
         <v>0</v>
@@ -1436,10 +1438,10 @@
         <v>0</v>
       </c>
       <c r="K20" t="n">
-        <v>74216</v>
+        <v>75236</v>
       </c>
       <c r="L20" t="n">
-        <v>2440</v>
+        <v>2479</v>
       </c>
       <c r="M20" t="n">
         <v>305259</v>
@@ -1463,19 +1465,19 @@
         <v>44034</v>
       </c>
       <c r="C21" t="n">
-        <v>99875</v>
+        <v>100483</v>
       </c>
       <c r="D21" t="n">
-        <v>7038</v>
+        <v>7063</v>
       </c>
       <c r="E21" t="n">
-        <v>13956</v>
+        <v>14038</v>
       </c>
       <c r="F21" t="n">
         <v>1484</v>
       </c>
       <c r="G21" t="n">
-        <v>30.06</v>
+        <v>29.99</v>
       </c>
       <c r="H21" t="n">
         <v>21.22</v>
@@ -1487,7 +1489,7 @@
         <v>1</v>
       </c>
       <c r="K21" t="n">
-        <v>46430</v>
+        <v>46806</v>
       </c>
       <c r="L21" t="n">
         <v>6992</v>
@@ -1558,20 +1560,20 @@
         </is>
       </c>
       <c r="B23" s="2" t="n">
-        <v>44033</v>
+        <v>44034</v>
       </c>
       <c r="C23" t="n">
-        <v>2712</v>
+        <v>2813</v>
       </c>
       <c r="D23" t="n">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E23" t="n">
         <v>15</v>
       </c>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="n">
-        <v>0.55</v>
+        <v>0.53</v>
       </c>
       <c r="H23" t="inlineStr"/>
       <c r="I23" t="b">
@@ -1601,7 +1603,7 @@
         </is>
       </c>
       <c r="B24" s="2" t="n">
-        <v>44033</v>
+        <v>44034</v>
       </c>
       <c r="C24" t="n">
         <v>1366</v>
@@ -1616,7 +1618,7 @@
         <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>11.38</v>
+        <v>11.39</v>
       </c>
       <c r="H24" t="n">
         <v>0</v>
@@ -1628,7 +1630,7 @@
         <v>1</v>
       </c>
       <c r="K24" t="n">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="L24" t="n">
         <v>56</v>
@@ -1652,25 +1654,25 @@
         </is>
       </c>
       <c r="B25" s="2" t="n">
-        <v>44032</v>
+        <v>44033</v>
       </c>
       <c r="C25" t="n">
-        <v>46116</v>
+        <v>46203</v>
       </c>
       <c r="D25" t="n">
         <v>3527</v>
       </c>
       <c r="E25" t="n">
-        <v>6312</v>
+        <v>6375</v>
       </c>
       <c r="F25" t="n">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="G25" t="n">
-        <v>13.69</v>
+        <v>13.8</v>
       </c>
       <c r="H25" t="n">
-        <v>18.49</v>
+        <v>18.46</v>
       </c>
       <c r="I25" t="b">
         <v>1</v>
@@ -1699,25 +1701,25 @@
         </is>
       </c>
       <c r="B26" s="2" t="n">
-        <v>44032</v>
+        <v>44034</v>
       </c>
       <c r="C26" t="n">
-        <v>23334</v>
+        <v>24104</v>
       </c>
       <c r="D26" t="n">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="E26" t="n">
-        <v>1734</v>
+        <v>1780</v>
       </c>
       <c r="F26" t="n">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G26" t="n">
-        <v>9.140000000000001</v>
+        <v>9.029999999999999</v>
       </c>
       <c r="H26" t="n">
-        <v>21.74</v>
+        <v>21.33</v>
       </c>
       <c r="I26" t="b">
         <v>0</v>
@@ -1726,10 +1728,10 @@
         <v>1</v>
       </c>
       <c r="K26" t="n">
-        <v>18962</v>
+        <v>19703</v>
       </c>
       <c r="L26" t="n">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="M26" t="n">
         <v>169801</v>
@@ -1750,25 +1752,25 @@
         </is>
       </c>
       <c r="B27" s="2" t="n">
-        <v>44033</v>
+        <v>44034</v>
       </c>
       <c r="C27" t="n">
-        <v>41059</v>
+        <v>41698</v>
       </c>
       <c r="D27" t="n">
-        <v>1763</v>
+        <v>1771</v>
       </c>
       <c r="E27" t="n">
-        <v>2012</v>
+        <v>2027</v>
       </c>
       <c r="F27" t="n">
         <v>118</v>
       </c>
       <c r="G27" t="n">
-        <v>6.19</v>
+        <v>6.17</v>
       </c>
       <c r="H27" t="n">
-        <v>6.92</v>
+        <v>6.89</v>
       </c>
       <c r="I27" t="b">
         <v>0</v>
@@ -1777,10 +1779,10 @@
         <v>0</v>
       </c>
       <c r="K27" t="n">
-        <v>32519</v>
+        <v>32858</v>
       </c>
       <c r="L27" t="n">
-        <v>1706</v>
+        <v>1713</v>
       </c>
       <c r="M27" t="n">
         <v>227938</v>
@@ -1852,25 +1854,25 @@
         </is>
       </c>
       <c r="B29" s="2" t="n">
-        <v>44033</v>
+        <v>44034</v>
       </c>
       <c r="C29" t="n">
-        <v>74637</v>
+        <v>75171</v>
       </c>
       <c r="D29" t="n">
-        <v>6051</v>
+        <v>6056</v>
       </c>
       <c r="E29" t="n">
-        <v>21478</v>
+        <v>21592</v>
       </c>
       <c r="F29" t="n">
-        <v>2411</v>
+        <v>2415</v>
       </c>
       <c r="G29" t="n">
-        <v>28.78</v>
+        <v>28.72</v>
       </c>
       <c r="H29" t="n">
-        <v>39.84</v>
+        <v>39.88</v>
       </c>
       <c r="I29" t="b">
         <v>1</v>
@@ -1899,25 +1901,25 @@
         </is>
       </c>
       <c r="B30" s="2" t="n">
-        <v>44027</v>
+        <v>44034</v>
       </c>
       <c r="C30" t="n">
-        <v>96583</v>
+        <v>99354</v>
       </c>
       <c r="D30" t="n">
-        <v>3498</v>
+        <v>3558</v>
       </c>
       <c r="E30" t="n">
-        <v>32137</v>
+        <v>36693</v>
       </c>
       <c r="F30" t="n">
-        <v>1724</v>
+        <v>1803</v>
       </c>
       <c r="G30" t="n">
-        <v>48.31</v>
+        <v>45.36</v>
       </c>
       <c r="H30" t="n">
-        <v>51.56</v>
+        <v>51.05</v>
       </c>
       <c r="I30" t="b">
         <v>0</v>
@@ -1926,10 +1928,10 @@
         <v>1</v>
       </c>
       <c r="K30" t="n">
-        <v>66518</v>
+        <v>80885</v>
       </c>
       <c r="L30" t="n">
-        <v>3344</v>
+        <v>3532</v>
       </c>
       <c r="M30" t="n">
         <v>1502916</v>
@@ -1950,25 +1952,25 @@
         </is>
       </c>
       <c r="B31" s="3" t="n">
-        <v>44032</v>
+        <v>44033</v>
       </c>
       <c r="C31" t="n">
-        <v>400769</v>
+        <v>413576</v>
       </c>
       <c r="D31" t="n">
-        <v>7755</v>
+        <v>7870</v>
       </c>
       <c r="E31" t="n">
-        <v>11069</v>
+        <v>11396</v>
       </c>
       <c r="F31" t="n">
-        <v>654</v>
+        <v>660</v>
       </c>
       <c r="G31" t="n">
-        <v>4.3</v>
+        <v>4.31</v>
       </c>
       <c r="H31" t="n">
-        <v>8.66</v>
+        <v>8.6</v>
       </c>
       <c r="I31" t="b">
         <v>0</v>
@@ -1977,10 +1979,10 @@
         <v>0</v>
       </c>
       <c r="K31" t="n">
-        <v>257550</v>
+        <v>264380</v>
       </c>
       <c r="L31" t="n">
-        <v>7555</v>
+        <v>7672</v>
       </c>
       <c r="M31" t="n">
         <v>2267875</v>
@@ -2001,22 +2003,22 @@
         </is>
       </c>
       <c r="B32" s="2" t="n">
-        <v>44033</v>
+        <v>44034</v>
       </c>
       <c r="C32" t="n">
-        <v>57916</v>
+        <v>58673</v>
       </c>
       <c r="D32" t="n">
-        <v>2652</v>
+        <v>2666</v>
       </c>
       <c r="E32" t="n">
-        <v>6651</v>
+        <v>6696</v>
       </c>
       <c r="F32" t="n">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="G32" t="n">
-        <v>11.48</v>
+        <v>11.41</v>
       </c>
       <c r="H32" t="n">
         <v>14.14</v>
@@ -2048,22 +2050,22 @@
         </is>
       </c>
       <c r="B33" s="2" t="n">
-        <v>44033</v>
+        <v>44034</v>
       </c>
       <c r="C33" t="n">
-        <v>2041</v>
+        <v>2132</v>
       </c>
       <c r="D33" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E33" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F33" t="n">
         <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>3.73</v>
+        <v>3.7</v>
       </c>
       <c r="H33" t="n">
         <v>0</v>
@@ -2075,7 +2077,7 @@
         <v>1</v>
       </c>
       <c r="K33" t="n">
-        <v>1287</v>
+        <v>1323</v>
       </c>
       <c r="L33" t="n">
         <v>18</v>
@@ -2099,25 +2101,25 @@
         </is>
       </c>
       <c r="B34" s="2" t="n">
-        <v>44033</v>
+        <v>44034</v>
       </c>
       <c r="C34" t="n">
-        <v>44135</v>
+        <v>44847</v>
       </c>
       <c r="D34" t="n">
-        <v>859</v>
+        <v>865</v>
       </c>
       <c r="E34" t="n">
-        <v>7019</v>
+        <v>7066</v>
       </c>
       <c r="F34" t="n">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G34" t="n">
-        <v>17.59</v>
+        <v>17.43</v>
       </c>
       <c r="H34" t="n">
-        <v>23.2</v>
+        <v>23.15</v>
       </c>
       <c r="I34" t="b">
         <v>0</v>
@@ -2126,10 +2128,10 @@
         <v>1</v>
       </c>
       <c r="K34" t="n">
-        <v>39895</v>
+        <v>40535</v>
       </c>
       <c r="L34" t="n">
-        <v>845</v>
+        <v>851</v>
       </c>
       <c r="M34" t="n">
         <v>368744</v>
@@ -2150,25 +2152,25 @@
         </is>
       </c>
       <c r="B35" s="2" t="n">
-        <v>44033</v>
+        <v>44034</v>
       </c>
       <c r="C35" t="n">
-        <v>148988</v>
+        <v>152302</v>
       </c>
       <c r="D35" t="n">
-        <v>3254</v>
+        <v>3335</v>
       </c>
       <c r="E35" t="n">
-        <v>38168</v>
+        <v>39406</v>
       </c>
       <c r="F35" t="n">
-        <v>1497</v>
+        <v>1525</v>
       </c>
       <c r="G35" t="n">
-        <v>25.62</v>
+        <v>25.87</v>
       </c>
       <c r="H35" t="n">
-        <v>46</v>
+        <v>45.73</v>
       </c>
       <c r="I35" t="b">
         <v>1</v>
@@ -2248,25 +2250,25 @@
         </is>
       </c>
       <c r="B37" s="2" t="n">
-        <v>44033</v>
+        <v>44034</v>
       </c>
       <c r="C37" t="n">
-        <v>6262</v>
+        <v>6295</v>
       </c>
       <c r="D37" t="n">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="E37" t="n">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="F37" t="n">
         <v>9</v>
       </c>
       <c r="G37" t="n">
-        <v>6</v>
+        <v>6.01</v>
       </c>
       <c r="H37" t="n">
-        <v>2.26</v>
+        <v>2.25</v>
       </c>
       <c r="I37" t="b">
         <v>0</v>
@@ -2275,10 +2277,10 @@
         <v>0</v>
       </c>
       <c r="K37" t="n">
-        <v>5349</v>
+        <v>5404</v>
       </c>
       <c r="L37" t="n">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="M37" t="n">
         <v>20516</v>
@@ -2427,13 +2429,13 @@
         <v>44034</v>
       </c>
       <c r="C41" t="n">
-        <v>39793</v>
+        <v>40000</v>
       </c>
       <c r="D41" t="n">
-        <v>808</v>
+        <v>811</v>
       </c>
       <c r="E41" t="n">
-        <v>3264</v>
+        <v>3280</v>
       </c>
       <c r="F41" t="n">
         <v>38</v>
@@ -2442,7 +2444,7 @@
         <v>8.199999999999999</v>
       </c>
       <c r="H41" t="n">
-        <v>4.7</v>
+        <v>4.69</v>
       </c>
       <c r="I41" t="b">
         <v>1</v>
@@ -2471,25 +2473,25 @@
         </is>
       </c>
       <c r="B42" s="2" t="n">
-        <v>44033</v>
+        <v>44034</v>
       </c>
       <c r="C42" t="n">
-        <v>102861</v>
+        <v>105001</v>
       </c>
       <c r="D42" t="n">
-        <v>1668</v>
+        <v>1698</v>
       </c>
       <c r="E42" t="n">
-        <v>16812</v>
+        <v>17314</v>
       </c>
       <c r="F42" t="n">
-        <v>530</v>
+        <v>536</v>
       </c>
       <c r="G42" t="n">
-        <v>23.98</v>
+        <v>23.99</v>
       </c>
       <c r="H42" t="n">
-        <v>32.9</v>
+        <v>32.66</v>
       </c>
       <c r="I42" t="b">
         <v>0</v>
@@ -2498,10 +2500,10 @@
         <v>1</v>
       </c>
       <c r="K42" t="n">
-        <v>70100</v>
+        <v>72174</v>
       </c>
       <c r="L42" t="n">
-        <v>1611</v>
+        <v>1641</v>
       </c>
       <c r="M42" t="n">
         <v>2179622</v>
@@ -2522,22 +2524,22 @@
         </is>
       </c>
       <c r="B43" s="2" t="n">
-        <v>44033</v>
+        <v>44034</v>
       </c>
       <c r="C43" t="n">
-        <v>163703</v>
+        <v>165301</v>
       </c>
       <c r="D43" t="n">
-        <v>7324</v>
+        <v>7347</v>
       </c>
       <c r="E43" t="n">
-        <v>27492</v>
+        <v>27704</v>
       </c>
       <c r="F43" t="n">
-        <v>2018</v>
+        <v>2024</v>
       </c>
       <c r="G43" t="n">
-        <v>16.79</v>
+        <v>16.76</v>
       </c>
       <c r="H43" t="n">
         <v>27.55</v>
@@ -2568,32 +2570,18 @@
           <t>Idaho</t>
         </is>
       </c>
-      <c r="B44" s="2" t="n">
-        <v>44033</v>
-      </c>
-      <c r="C44" t="n">
-        <v>15822</v>
-      </c>
-      <c r="D44" t="n">
-        <v>123</v>
-      </c>
-      <c r="E44" t="n">
-        <v>201</v>
-      </c>
-      <c r="F44" t="n">
-        <v>1</v>
-      </c>
-      <c r="G44" t="n">
-        <v>1.27</v>
-      </c>
-      <c r="H44" t="n">
-        <v>0.8100000000000001</v>
-      </c>
+      <c r="B44" t="inlineStr"/>
+      <c r="C44" t="inlineStr"/>
+      <c r="D44" t="inlineStr"/>
+      <c r="E44" t="inlineStr"/>
+      <c r="F44" t="inlineStr"/>
+      <c r="G44" t="inlineStr"/>
+      <c r="H44" t="inlineStr"/>
       <c r="I44" t="b">
         <v>0</v>
       </c>
       <c r="J44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K44" t="inlineStr"/>
       <c r="L44" t="inlineStr"/>
@@ -2605,7 +2593,7 @@
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Success!</t>
+          <t>An error occurred. ... TimeoutException('', None, None)</t>
         </is>
       </c>
     </row>
@@ -2616,25 +2604,25 @@
         </is>
       </c>
       <c r="B45" s="2" t="n">
-        <v>44033</v>
+        <v>44034</v>
       </c>
       <c r="C45" t="n">
-        <v>47457</v>
+        <v>47961</v>
       </c>
       <c r="D45" t="n">
-        <v>1548</v>
+        <v>1552</v>
       </c>
       <c r="E45" t="n">
-        <v>9345</v>
+        <v>9842</v>
       </c>
       <c r="F45" t="n">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G45" t="n">
-        <v>19.69</v>
+        <v>20.52</v>
       </c>
       <c r="H45" t="n">
-        <v>9.75</v>
+        <v>9.789999999999999</v>
       </c>
       <c r="I45" t="b">
         <v>1</v>
@@ -2663,16 +2651,16 @@
         </is>
       </c>
       <c r="B46" s="2" t="n">
-        <v>44033</v>
+        <v>44034</v>
       </c>
       <c r="C46" t="n">
-        <v>114033</v>
+        <v>114320</v>
       </c>
       <c r="D46" t="n">
-        <v>8450</v>
+        <v>8468</v>
       </c>
       <c r="E46" t="n">
-        <v>10704</v>
+        <v>10731</v>
       </c>
       <c r="F46" t="n">
         <v>693</v>
@@ -2681,7 +2669,7 @@
         <v>9.390000000000001</v>
       </c>
       <c r="H46" t="n">
-        <v>8.199999999999999</v>
+        <v>8.18</v>
       </c>
       <c r="I46" t="b">
         <v>1</v>
@@ -2710,25 +2698,25 @@
         </is>
       </c>
       <c r="B47" s="2" t="n">
-        <v>44033</v>
+        <v>44034</v>
       </c>
       <c r="C47" t="n">
-        <v>16555</v>
+        <v>16911</v>
       </c>
       <c r="D47" t="n">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="E47" t="n">
-        <v>4693</v>
+        <v>4771</v>
       </c>
       <c r="F47" t="n">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G47" t="n">
-        <v>30.57</v>
+        <v>30.42</v>
       </c>
       <c r="H47" t="n">
-        <v>39.78</v>
+        <v>39.73</v>
       </c>
       <c r="I47" t="b">
         <v>0</v>
@@ -2737,10 +2725,10 @@
         <v>0</v>
       </c>
       <c r="K47" t="n">
-        <v>15354</v>
+        <v>15682</v>
       </c>
       <c r="L47" t="n">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="M47" t="n">
         <v>252321</v>
@@ -2761,25 +2749,25 @@
         </is>
       </c>
       <c r="B48" s="2" t="n">
-        <v>44033</v>
+        <v>44034</v>
       </c>
       <c r="C48" t="n">
-        <v>34760</v>
+        <v>36063</v>
       </c>
       <c r="D48" t="n">
-        <v>1143</v>
+        <v>1159</v>
       </c>
       <c r="E48" t="n">
-        <v>7939</v>
+        <v>8118</v>
       </c>
       <c r="F48" t="n">
-        <v>384</v>
+        <v>389</v>
       </c>
       <c r="G48" t="n">
-        <v>31.99</v>
+        <v>31.68</v>
       </c>
       <c r="H48" t="n">
-        <v>36.06</v>
+        <v>36.22</v>
       </c>
       <c r="I48" t="b">
         <v>0</v>
@@ -2788,10 +2776,10 @@
         <v>1</v>
       </c>
       <c r="K48" t="n">
-        <v>24820</v>
+        <v>25629</v>
       </c>
       <c r="L48" t="n">
-        <v>1065</v>
+        <v>1074</v>
       </c>
       <c r="M48" t="n">
         <v>704896</v>

</xml_diff>

<commit_message>
Results from July 22, 2020 04:16:57 PM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-22.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-22.xlsx
@@ -1262,25 +1262,25 @@
         </is>
       </c>
       <c r="B17" s="2" t="n">
-        <v>44032</v>
+        <v>44033</v>
       </c>
       <c r="C17" t="n">
-        <v>161673</v>
+        <v>164870</v>
       </c>
       <c r="D17" t="n">
-        <v>4154</v>
+        <v>4213</v>
       </c>
       <c r="E17" t="n">
-        <v>4308</v>
+        <v>4391</v>
       </c>
       <c r="F17" t="n">
-        <v>413</v>
+        <v>419</v>
       </c>
       <c r="G17" t="n">
         <v>4.64</v>
       </c>
       <c r="H17" t="n">
-        <v>10.68</v>
+        <v>10.67</v>
       </c>
       <c r="I17" t="b">
         <v>0</v>
@@ -1289,10 +1289,10 @@
         <v>0</v>
       </c>
       <c r="K17" t="n">
-        <v>92881</v>
+        <v>94674</v>
       </c>
       <c r="L17" t="n">
-        <v>3867</v>
+        <v>3927</v>
       </c>
       <c r="M17" t="n">
         <v>823987</v>
@@ -2370,7 +2370,7 @@
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>An error occurred. ... AttributeError("'numpy.float64' object has no attribute 'split'")</t>
+          <t>An error occurred. ... HTTPError('504 Server Error: Gateway Time-out for url: https://myhealthycommunity.dhss.delaware.gov/locations/state/')</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Results from July 22, 2020 04:26:17 PM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-22.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-22.xlsx
@@ -1803,25 +1803,25 @@
         </is>
       </c>
       <c r="B28" s="2" t="n">
-        <v>44033</v>
+        <v>44034</v>
       </c>
       <c r="C28" t="n">
-        <v>23190</v>
+        <v>23486</v>
       </c>
       <c r="D28" t="n">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="E28" t="n">
-        <v>1369</v>
+        <v>1390</v>
       </c>
       <c r="F28" t="n">
         <v>23</v>
       </c>
       <c r="G28" t="n">
-        <v>7.61</v>
+        <v>7.65</v>
       </c>
       <c r="H28" t="n">
-        <v>7.67</v>
+        <v>7.74</v>
       </c>
       <c r="I28" t="b">
         <v>0</v>
@@ -1830,10 +1830,10 @@
         <v>1</v>
       </c>
       <c r="K28" t="n">
-        <v>17993</v>
+        <v>18180</v>
       </c>
       <c r="L28" t="n">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="M28" t="n">
         <v>90860</v>
@@ -2429,13 +2429,13 @@
         <v>44034</v>
       </c>
       <c r="C41" t="n">
-        <v>40000</v>
+        <v>40085</v>
       </c>
       <c r="D41" t="n">
         <v>811</v>
       </c>
       <c r="E41" t="n">
-        <v>3280</v>
+        <v>3286</v>
       </c>
       <c r="F41" t="n">
         <v>38</v>
@@ -2570,18 +2570,32 @@
           <t>Idaho</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr"/>
-      <c r="C44" t="inlineStr"/>
-      <c r="D44" t="inlineStr"/>
-      <c r="E44" t="inlineStr"/>
-      <c r="F44" t="inlineStr"/>
-      <c r="G44" t="inlineStr"/>
-      <c r="H44" t="inlineStr"/>
+      <c r="B44" s="2" t="n">
+        <v>44034</v>
+      </c>
+      <c r="C44" t="n">
+        <v>16322</v>
+      </c>
+      <c r="D44" t="n">
+        <v>131</v>
+      </c>
+      <c r="E44" t="n">
+        <v>208</v>
+      </c>
+      <c r="F44" t="n">
+        <v>2</v>
+      </c>
+      <c r="G44" t="n">
+        <v>1.27</v>
+      </c>
+      <c r="H44" t="n">
+        <v>1.53</v>
+      </c>
       <c r="I44" t="b">
         <v>0</v>
       </c>
       <c r="J44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K44" t="inlineStr"/>
       <c r="L44" t="inlineStr"/>
@@ -2593,7 +2607,7 @@
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>An error occurred. ... TimeoutException('', None, None)</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Results from July 22, 2020 04:46:03 PM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-22.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-22.xlsx
@@ -2199,25 +2199,25 @@
         </is>
       </c>
       <c r="B36" s="2" t="n">
-        <v>44033</v>
+        <v>44034</v>
       </c>
       <c r="C36" t="n">
-        <v>48575</v>
+        <v>49247</v>
       </c>
       <c r="D36" t="n">
-        <v>1465</v>
+        <v>1468</v>
       </c>
       <c r="E36" t="n">
-        <v>1732</v>
+        <v>1743</v>
       </c>
       <c r="F36" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G36" t="n">
         <v>5.44</v>
       </c>
       <c r="H36" t="n">
-        <v>3.42</v>
+        <v>3.47</v>
       </c>
       <c r="I36" t="b">
         <v>0</v>
@@ -2226,10 +2226,10 @@
         <v>0</v>
       </c>
       <c r="K36" t="n">
-        <v>31843</v>
+        <v>32066</v>
       </c>
       <c r="L36" t="n">
-        <v>1403</v>
+        <v>1413</v>
       </c>
       <c r="M36" t="n">
         <v>269854</v>
@@ -2370,7 +2370,7 @@
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>An error occurred. ... HTTPError('504 Server Error: Gateway Time-out for url: https://myhealthycommunity.dhss.delaware.gov/locations/state/')</t>
+          <t>An error occurred. ... AttributeError("'numpy.float64' object has no attribute 'split'")</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Results from July 22, 2020 04:55:58 PM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-22.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-22.xlsx
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>44033</v>
+        <v>44034</v>
       </c>
       <c r="C3" t="n">
         <v>31867</v>
@@ -622,43 +622,21 @@
           <t>New York -- New York</t>
         </is>
       </c>
-      <c r="B4" s="2" t="n">
-        <v>44034</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>219128</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>18803</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>33790</v>
-      </c>
-      <c r="F4" t="n">
-        <v>5239</v>
-      </c>
-      <c r="G4" t="n">
-        <v>30.07</v>
-      </c>
-      <c r="H4" t="n">
-        <v>30.43</v>
-      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
       <c r="I4" t="b">
         <v>0</v>
       </c>
       <c r="J4" t="b">
-        <v>1</v>
-      </c>
-      <c r="K4" t="n">
-        <v>112360</v>
-      </c>
-      <c r="L4" t="n">
-        <v>17217</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
       <c r="M4" t="n">
         <v>2049418</v>
       </c>
@@ -667,7 +645,7 @@
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Success!</t>
+          <t>An error occurred. ... RateLimitExceededException(403, {'message': "API rate limit exceeded for 132.145.200.60. (But here's the good news: Authenticated requests get a higher rate limit. Check out the documentation for more details.)", 'documentation_url': 'https://developer.github.com/v3/#rate-limiting'})</t>
         </is>
       </c>
     </row>
@@ -2370,7 +2348,7 @@
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>An error occurred. ... AttributeError("'numpy.float64' object has no attribute 'split'")</t>
+          <t>An error occurred. ... HTTPError('504 Server Error: Gateway Time-out for url: https://myhealthycommunity.dhss.delaware.gov/locations/state/')</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Results from July 22, 2020 05:06:38 PM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-22.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-22.xlsx
@@ -575,10 +575,10 @@
         <v>44034</v>
       </c>
       <c r="C3" t="n">
-        <v>31867</v>
+        <v>33555</v>
       </c>
       <c r="D3" t="n">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="E3" t="n">
         <v>464</v>
@@ -622,21 +622,43 @@
           <t>New York -- New York</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
+      <c r="B4" s="2" t="n">
+        <v>44034</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>219128</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>18803</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>33790</v>
+      </c>
+      <c r="F4" t="n">
+        <v>5239</v>
+      </c>
+      <c r="G4" t="n">
+        <v>30.07</v>
+      </c>
+      <c r="H4" t="n">
+        <v>30.43</v>
+      </c>
       <c r="I4" t="b">
         <v>0</v>
       </c>
       <c r="J4" t="b">
-        <v>0</v>
-      </c>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K4" t="n">
+        <v>112360</v>
+      </c>
+      <c r="L4" t="n">
+        <v>17217</v>
+      </c>
       <c r="M4" t="n">
         <v>2049418</v>
       </c>
@@ -645,7 +667,7 @@
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>An error occurred. ... RateLimitExceededException(403, {'message': "API rate limit exceeded for 132.145.200.60. (But here's the good news: Authenticated requests get a higher rate limit. Check out the documentation for more details.)", 'documentation_url': 'https://developer.github.com/v3/#rate-limiting'})</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
@@ -958,25 +980,25 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>44033</v>
+        <v>44034</v>
       </c>
       <c r="C11" t="n">
-        <v>24520</v>
+        <v>25107</v>
       </c>
       <c r="D11" t="n">
-        <v>487</v>
+        <v>505</v>
       </c>
       <c r="E11" t="n">
-        <v>895</v>
+        <v>918</v>
       </c>
       <c r="F11" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G11" t="n">
-        <v>4.69</v>
+        <v>4.67</v>
       </c>
       <c r="H11" t="n">
-        <v>3.74</v>
+        <v>3.85</v>
       </c>
       <c r="I11" t="b">
         <v>0</v>
@@ -985,10 +1007,10 @@
         <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>19099</v>
+        <v>19655</v>
       </c>
       <c r="L11" t="n">
-        <v>481</v>
+        <v>493</v>
       </c>
       <c r="M11" t="n">
         <v>166412</v>

</xml_diff>

<commit_message>
Results from July 22, 2020 05:26:29 PM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-22.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-22.xlsx
@@ -932,22 +932,22 @@
         <v>44034</v>
       </c>
       <c r="C10" t="n">
-        <v>34655</v>
+        <v>35246</v>
       </c>
       <c r="D10" t="n">
-        <v>374</v>
+        <v>380</v>
       </c>
       <c r="E10" t="n">
-        <v>7364</v>
+        <v>7521</v>
       </c>
       <c r="F10" t="n">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G10" t="n">
-        <v>24.62</v>
+        <v>24.57</v>
       </c>
       <c r="H10" t="n">
-        <v>26.61</v>
+        <v>26.53</v>
       </c>
       <c r="I10" t="b">
         <v>0</v>
@@ -956,10 +956,10 @@
         <v>1</v>
       </c>
       <c r="K10" t="n">
-        <v>29915</v>
+        <v>30608</v>
       </c>
       <c r="L10" t="n">
-        <v>372</v>
+        <v>377</v>
       </c>
       <c r="M10" t="n">
         <v>460970</v>
@@ -2432,10 +2432,10 @@
         <v>40085</v>
       </c>
       <c r="D41" t="n">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="E41" t="n">
-        <v>3286</v>
+        <v>3287</v>
       </c>
       <c r="F41" t="n">
         <v>38</v>
@@ -2444,7 +2444,7 @@
         <v>8.199999999999999</v>
       </c>
       <c r="H41" t="n">
-        <v>4.69</v>
+        <v>4.68</v>
       </c>
       <c r="I41" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Results from July 22, 2020 05:56:00 PM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-22.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-22.xlsx
@@ -622,43 +622,21 @@
           <t>New York -- New York</t>
         </is>
       </c>
-      <c r="B4" s="2" t="n">
-        <v>44034</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>219128</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>18803</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>33790</v>
-      </c>
-      <c r="F4" t="n">
-        <v>5239</v>
-      </c>
-      <c r="G4" t="n">
-        <v>30.07</v>
-      </c>
-      <c r="H4" t="n">
-        <v>30.43</v>
-      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
       <c r="I4" t="b">
         <v>0</v>
       </c>
       <c r="J4" t="b">
-        <v>1</v>
-      </c>
-      <c r="K4" t="n">
-        <v>112360</v>
-      </c>
-      <c r="L4" t="n">
-        <v>17217</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
       <c r="M4" t="n">
         <v>2049418</v>
       </c>
@@ -667,7 +645,7 @@
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Success!</t>
+          <t>An error occurred. ... RateLimitExceededException(403, {'message': "API rate limit exceeded for 132.145.200.60. (But here's the good news: Authenticated requests get a higher rate limit. Check out the documentation for more details.)", 'documentation_url': 'https://developer.github.com/v3/#rate-limiting'})</t>
         </is>
       </c>
     </row>
@@ -2370,7 +2348,7 @@
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>An error occurred. ... HTTPError('504 Server Error: Gateway Time-out for url: https://myhealthycommunity.dhss.delaware.gov/locations/state/')</t>
+          <t>An error occurred. ... AttributeError("'numpy.float64' object has no attribute 'split'")</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Results from July 22, 2020 06:19:03 PM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-22.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-22.xlsx
@@ -622,21 +622,43 @@
           <t>New York -- New York</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
+      <c r="B4" s="2" t="n">
+        <v>44034</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>219128</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>18803</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>33790</v>
+      </c>
+      <c r="F4" t="n">
+        <v>5239</v>
+      </c>
+      <c r="G4" t="n">
+        <v>30.07</v>
+      </c>
+      <c r="H4" t="n">
+        <v>30.43</v>
+      </c>
       <c r="I4" t="b">
         <v>0</v>
       </c>
       <c r="J4" t="b">
-        <v>0</v>
-      </c>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K4" t="n">
+        <v>112360</v>
+      </c>
+      <c r="L4" t="n">
+        <v>17217</v>
+      </c>
       <c r="M4" t="n">
         <v>2049418</v>
       </c>
@@ -645,7 +667,7 @@
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>An error occurred. ... RateLimitExceededException(403, {'message': "API rate limit exceeded for 132.145.200.60. (But here's the good news: Authenticated requests get a higher rate limit. Check out the documentation for more details.)", 'documentation_url': 'https://developer.github.com/v3/#rate-limiting'})</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
@@ -2413,7 +2435,7 @@
         <v>812</v>
       </c>
       <c r="E41" t="n">
-        <v>3287</v>
+        <v>3288</v>
       </c>
       <c r="F41" t="n">
         <v>38</v>

</xml_diff>

<commit_message>
Results from July 22, 2020 07:07:30 PM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-22.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-22.xlsx
@@ -622,43 +622,21 @@
           <t>New York -- New York</t>
         </is>
       </c>
-      <c r="B4" s="2" t="n">
-        <v>44034</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>219128</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>18803</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>33790</v>
-      </c>
-      <c r="F4" t="n">
-        <v>5239</v>
-      </c>
-      <c r="G4" t="n">
-        <v>30.07</v>
-      </c>
-      <c r="H4" t="n">
-        <v>30.43</v>
-      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
       <c r="I4" t="b">
         <v>0</v>
       </c>
       <c r="J4" t="b">
-        <v>1</v>
-      </c>
-      <c r="K4" t="n">
-        <v>112360</v>
-      </c>
-      <c r="L4" t="n">
-        <v>17217</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
       <c r="M4" t="n">
         <v>2049418</v>
       </c>
@@ -667,7 +645,7 @@
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Success!</t>
+          <t>An error occurred. ... RateLimitExceededException(403, {'message': "API rate limit exceeded for 132.145.200.60. (But here's the good news: Authenticated requests get a higher rate limit. Check out the documentation for more details.)", 'documentation_url': 'https://developer.github.com/v3/#rate-limiting'})</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Results from July 22, 2020 07:43:29 PM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-22.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-22.xlsx
@@ -622,21 +622,43 @@
           <t>New York -- New York</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
+      <c r="B4" s="2" t="n">
+        <v>44034</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>219128</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>18803</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>33790</v>
+      </c>
+      <c r="F4" t="n">
+        <v>5239</v>
+      </c>
+      <c r="G4" t="n">
+        <v>30.07</v>
+      </c>
+      <c r="H4" t="n">
+        <v>30.43</v>
+      </c>
       <c r="I4" t="b">
         <v>0</v>
       </c>
       <c r="J4" t="b">
-        <v>0</v>
-      </c>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K4" t="n">
+        <v>112360</v>
+      </c>
+      <c r="L4" t="n">
+        <v>17217</v>
+      </c>
       <c r="M4" t="n">
         <v>2049418</v>
       </c>
@@ -645,7 +667,7 @@
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>An error occurred. ... RateLimitExceededException(403, {'message': "API rate limit exceeded for 132.145.200.60. (But here's the good news: Authenticated requests get a higher rate limit. Check out the documentation for more details.)", 'documentation_url': 'https://developer.github.com/v3/#rate-limiting'})</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
@@ -2407,19 +2429,19 @@
         <v>44034</v>
       </c>
       <c r="C41" t="n">
-        <v>40085</v>
+        <v>40146</v>
       </c>
       <c r="D41" t="n">
         <v>812</v>
       </c>
       <c r="E41" t="n">
-        <v>3288</v>
+        <v>3289</v>
       </c>
       <c r="F41" t="n">
         <v>38</v>
       </c>
       <c r="G41" t="n">
-        <v>8.199999999999999</v>
+        <v>8.19</v>
       </c>
       <c r="H41" t="n">
         <v>4.68</v>
@@ -2548,32 +2570,18 @@
           <t>Idaho</t>
         </is>
       </c>
-      <c r="B44" s="2" t="n">
-        <v>44034</v>
-      </c>
-      <c r="C44" t="n">
-        <v>16322</v>
-      </c>
-      <c r="D44" t="n">
-        <v>131</v>
-      </c>
-      <c r="E44" t="n">
-        <v>208</v>
-      </c>
-      <c r="F44" t="n">
-        <v>2</v>
-      </c>
-      <c r="G44" t="n">
-        <v>1.27</v>
-      </c>
-      <c r="H44" t="n">
-        <v>1.53</v>
-      </c>
+      <c r="B44" t="inlineStr"/>
+      <c r="C44" t="inlineStr"/>
+      <c r="D44" t="inlineStr"/>
+      <c r="E44" t="inlineStr"/>
+      <c r="F44" t="inlineStr"/>
+      <c r="G44" t="inlineStr"/>
+      <c r="H44" t="inlineStr"/>
       <c r="I44" t="b">
         <v>0</v>
       </c>
       <c r="J44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K44" t="inlineStr"/>
       <c r="L44" t="inlineStr"/>
@@ -2585,7 +2593,7 @@
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Success!</t>
+          <t>An error occurred. ... TimeoutException('', None, None)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Results from July 22, 2020 08:15:55 PM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-22.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-22.xlsx
@@ -2570,18 +2570,32 @@
           <t>Idaho</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr"/>
-      <c r="C44" t="inlineStr"/>
-      <c r="D44" t="inlineStr"/>
-      <c r="E44" t="inlineStr"/>
-      <c r="F44" t="inlineStr"/>
-      <c r="G44" t="inlineStr"/>
-      <c r="H44" t="inlineStr"/>
+      <c r="B44" s="2" t="n">
+        <v>44034</v>
+      </c>
+      <c r="C44" t="n">
+        <v>16322</v>
+      </c>
+      <c r="D44" t="n">
+        <v>131</v>
+      </c>
+      <c r="E44" t="n">
+        <v>208</v>
+      </c>
+      <c r="F44" t="n">
+        <v>2</v>
+      </c>
+      <c r="G44" t="n">
+        <v>1.27</v>
+      </c>
+      <c r="H44" t="n">
+        <v>1.53</v>
+      </c>
       <c r="I44" t="b">
         <v>0</v>
       </c>
       <c r="J44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K44" t="inlineStr"/>
       <c r="L44" t="inlineStr"/>
@@ -2593,7 +2607,7 @@
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>An error occurred. ... TimeoutException('', None, None)</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Results from July 22, 2020 08:22:59 PM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-22.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-22.xlsx
@@ -2370,7 +2370,7 @@
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>An error occurred. ... HTTPError('504 Server Error: Gateway Time-out for url: https://myhealthycommunity.dhss.delaware.gov/locations/state/')</t>
+          <t>An error occurred. ... AttributeError("'numpy.float64' object has no attribute 'split'")</t>
         </is>
       </c>
     </row>
@@ -2429,19 +2429,19 @@
         <v>44034</v>
       </c>
       <c r="C41" t="n">
-        <v>40146</v>
+        <v>40208</v>
       </c>
       <c r="D41" t="n">
         <v>812</v>
       </c>
       <c r="E41" t="n">
-        <v>3289</v>
+        <v>3291</v>
       </c>
       <c r="F41" t="n">
         <v>38</v>
       </c>
       <c r="G41" t="n">
-        <v>8.19</v>
+        <v>8.18</v>
       </c>
       <c r="H41" t="n">
         <v>4.68</v>

</xml_diff>